<commit_message>
Update of Rachel setup
</commit_message>
<xml_diff>
--- a/Domain setup/NoFlow_Boundaries.xlsx
+++ b/Domain setup/NoFlow_Boundaries.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/Teaching/Groundwater_Modeling/HWRS582_Spring20/Course_Mat_Git/FInal_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelspinti/Documents/HWRS_582/Aguaseca_Project/Domain setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB07EDC-37C5-8E44-9F0E-9466FD6C2E52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004DA971-D249-7747-A80A-FB61A3A6B31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27900" yWindow="460" windowWidth="29900" windowHeight="28040" xr2:uid="{76ED07CC-4216-B149-B9A3-8A78C10F09A5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{76ED07CC-4216-B149-B9A3-8A78C10F09A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7613CA-5890-FD4E-9AAB-B1452D4EB631}">
   <dimension ref="A1:AY57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3494,6 +3494,158 @@
       <c r="AX52" s="8"/>
       <c r="AY52" s="4"/>
     </row>
+    <row r="53" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>5</v>
+      </c>
+      <c r="G53">
+        <v>6</v>
+      </c>
+      <c r="H53">
+        <v>7</v>
+      </c>
+      <c r="I53">
+        <v>8</v>
+      </c>
+      <c r="J53">
+        <v>9</v>
+      </c>
+      <c r="K53">
+        <v>10</v>
+      </c>
+      <c r="L53">
+        <v>11</v>
+      </c>
+      <c r="M53">
+        <v>12</v>
+      </c>
+      <c r="N53">
+        <v>13</v>
+      </c>
+      <c r="O53">
+        <v>14</v>
+      </c>
+      <c r="P53">
+        <v>15</v>
+      </c>
+      <c r="Q53">
+        <v>16</v>
+      </c>
+      <c r="R53">
+        <v>17</v>
+      </c>
+      <c r="S53">
+        <v>18</v>
+      </c>
+      <c r="T53">
+        <v>19</v>
+      </c>
+      <c r="U53">
+        <v>20</v>
+      </c>
+      <c r="V53">
+        <v>21</v>
+      </c>
+      <c r="W53">
+        <v>22</v>
+      </c>
+      <c r="X53">
+        <v>23</v>
+      </c>
+      <c r="Y53">
+        <v>24</v>
+      </c>
+      <c r="Z53">
+        <v>25</v>
+      </c>
+      <c r="AA53">
+        <v>26</v>
+      </c>
+      <c r="AB53">
+        <v>27</v>
+      </c>
+      <c r="AC53">
+        <v>28</v>
+      </c>
+      <c r="AD53">
+        <v>29</v>
+      </c>
+      <c r="AE53">
+        <v>30</v>
+      </c>
+      <c r="AF53">
+        <v>31</v>
+      </c>
+      <c r="AG53">
+        <v>32</v>
+      </c>
+      <c r="AH53">
+        <v>33</v>
+      </c>
+      <c r="AI53">
+        <v>34</v>
+      </c>
+      <c r="AJ53">
+        <v>35</v>
+      </c>
+      <c r="AK53">
+        <v>36</v>
+      </c>
+      <c r="AL53">
+        <v>37</v>
+      </c>
+      <c r="AM53">
+        <v>38</v>
+      </c>
+      <c r="AN53">
+        <v>39</v>
+      </c>
+      <c r="AO53">
+        <v>40</v>
+      </c>
+      <c r="AP53">
+        <v>41</v>
+      </c>
+      <c r="AQ53">
+        <v>42</v>
+      </c>
+      <c r="AR53">
+        <v>43</v>
+      </c>
+      <c r="AS53">
+        <v>44</v>
+      </c>
+      <c r="AT53">
+        <v>45</v>
+      </c>
+      <c r="AU53">
+        <v>46</v>
+      </c>
+      <c r="AV53">
+        <v>47</v>
+      </c>
+      <c r="AW53">
+        <v>48</v>
+      </c>
+      <c r="AX53">
+        <v>49</v>
+      </c>
+      <c r="AY53">
+        <v>50</v>
+      </c>
+    </row>
     <row r="55" spans="1:51" x14ac:dyDescent="0.2">
       <c r="B55" s="14"/>
       <c r="C55" t="s">

</xml_diff>